<commit_message>
added order, data pages duplicating from game page to start.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Ant-Vue\ZCool-live-broadcast-systemdev-\1.docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9492" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
   <si>
     <t>Transitional backend</t>
   </si>
@@ -354,9 +359,6 @@
   </si>
   <si>
     <t>site exist</t>
-  </si>
-  <si>
-    <t>Developed by junn</t>
   </si>
   <si>
     <t>both exist</t>
@@ -371,18 +373,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -399,163 +395,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1A1A1A"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,13 +422,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.25"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,198 +446,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -793,251 +459,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1072,12 +496,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1099,62 +517,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1412,220 +792,218 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88888888888889" style="15"/>
-    <col min="2" max="2" width="37.3333333333333" style="15" customWidth="1"/>
-    <col min="3" max="3" width="24.5555555555556" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.88888888888889" style="15"/>
+    <col min="1" max="1" width="8.88671875" style="13"/>
+    <col min="2" max="2" width="37.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:3">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
-      <c r="C5" s="16" t="s">
+    <row r="5" spans="2:3">
+      <c r="C5" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="16" t="s">
+    <row r="6" spans="2:3">
+      <c r="C6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:3">
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="2:3">
+      <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:3">
-      <c r="C8" s="16" t="s">
+    <row r="8" spans="2:3">
+      <c r="C8" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:3">
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="2:3">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:3">
-      <c r="C10" s="16" t="s">
+    <row r="10" spans="2:3">
+      <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="3:3">
-      <c r="C14" s="16" t="s">
+    <row r="14" spans="2:3">
+      <c r="C14" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:3">
-      <c r="C15" s="16" t="s">
+    <row r="15" spans="2:3">
+      <c r="C15" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:3">
-      <c r="C16" s="16" t="s">
+    <row r="16" spans="2:3">
+      <c r="C16" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="16" t="s">
+    <row r="17" spans="2:3">
+      <c r="C17" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="16" t="s">
+    <row r="18" spans="2:3">
+      <c r="C18" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="16" t="s">
+    <row r="19" spans="2:3">
+      <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="16" t="s">
+    <row r="20" spans="2:3">
+      <c r="C20" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
-      <c r="C21" s="16" t="s">
+    <row r="21" spans="2:3">
+      <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="15" t="s">
+    <row r="22" spans="2:3">
+      <c r="B22" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="3:3">
-      <c r="C26" s="16" t="s">
+    <row r="26" spans="2:3">
+      <c r="C26" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="17" t="s">
+    <row r="27" spans="2:3">
+      <c r="B27" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="15" t="s">
+    <row r="28" spans="2:3">
+      <c r="B28" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="17" t="s">
+    <row r="29" spans="2:3">
+      <c r="B29" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="18" t="s">
+    <row r="33" spans="2:3">
+      <c r="C33" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
-      <c r="C34" s="18" t="s">
+    <row r="34" spans="2:3">
+      <c r="C34" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="17" t="s">
+    <row r="35" spans="2:3">
+      <c r="B35" s="15" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="19.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="15.2222222222222" customWidth="1"/>
-    <col min="5" max="5" width="26.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="15.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="1" customFormat="1" spans="1:3">
+    <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1636,7 +1014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:5">
+    <row r="3" spans="1:5" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1653,7 +1031,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="2:5">
+    <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
@@ -1663,7 +1041,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1675,7 +1053,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:3">
+    <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1686,7 +1064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:5">
+    <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1703,7 +1081,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" spans="2:5">
+    <row r="8" spans="1:5" s="1" customFormat="1">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
@@ -1713,7 +1091,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:3">
+    <row r="9" spans="1:5" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1724,7 +1102,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1735,7 +1113,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:3">
+    <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1746,40 +1124,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
+    <row r="12" spans="1:5" s="12" customFormat="1">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" spans="1:3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:5" s="12" customFormat="1">
+      <c r="A13" s="12">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
+    <row r="14" spans="1:5" s="12" customFormat="1">
+      <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="1" spans="1:3">
+    <row r="15" spans="1:5" s="3" customFormat="1">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1790,7 +1168,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" s="3" customFormat="1" spans="1:3">
+    <row r="16" spans="1:5" s="3" customFormat="1">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1801,18 +1179,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="1" spans="1:3">
-      <c r="A17" s="3">
+    <row r="17" spans="1:5" s="12" customFormat="1">
+      <c r="A17" s="12">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1823,7 +1201,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1834,7 +1212,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:3">
+    <row r="20" spans="1:5" s="1" customFormat="1">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1845,7 +1223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1856,7 +1234,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="1" spans="1:5">
+    <row r="22" spans="1:5" s="1" customFormat="1">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1873,15 +1251,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" spans="4:5">
-      <c r="D23" s="12" t="s">
+    <row r="23" spans="1:5" s="1" customFormat="1">
+      <c r="D23" s="10" t="s">
         <v>76</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" spans="4:5">
+    <row r="24" spans="1:5" s="1" customFormat="1">
       <c r="D24" s="1" t="s">
         <v>78</v>
       </c>
@@ -1889,7 +1267,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="4:5">
+    <row r="25" spans="1:5" s="1" customFormat="1">
       <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
@@ -1897,7 +1275,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="4:5">
+    <row r="26" spans="1:5" s="1" customFormat="1">
       <c r="D26" s="1" t="s">
         <v>81</v>
       </c>
@@ -1905,7 +1283,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="1" spans="4:5">
+    <row r="27" spans="1:5" s="1" customFormat="1">
       <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
@@ -1913,7 +1291,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="1" spans="1:5">
+    <row r="28" spans="1:5" s="1" customFormat="1">
       <c r="A28" s="1">
         <v>20</v>
       </c>
@@ -1930,7 +1308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" s="1" customFormat="1" spans="4:5">
+    <row r="29" spans="1:5" s="1" customFormat="1">
       <c r="D29" s="1" t="s">
         <v>88</v>
       </c>
@@ -1938,7 +1316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" s="1" customFormat="1" spans="4:5">
+    <row r="30" spans="1:5" s="1" customFormat="1">
       <c r="D30" s="1" t="s">
         <v>89</v>
       </c>
@@ -1947,158 +1325,155 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="13">
+      <c r="A31" s="11">
         <v>21</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="13">
+      <c r="A33" s="11">
         <v>22</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="13">
+      <c r="A35" s="11">
         <v>23</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="13">
+      <c r="A38" s="11">
         <v>24</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="14" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed components in analysis page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -12,99 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
-  <si>
-    <t>Transitional backend</t>
-  </si>
-  <si>
-    <t>Official backstage login</t>
-  </si>
-  <si>
-    <t>Data Overview</t>
-  </si>
-  <si>
-    <t>User data display</t>
-  </si>
-  <si>
-    <t>User data curve chart</t>
-  </si>
-  <si>
-    <t>User section</t>
-  </si>
-  <si>
-    <t>Transaction amount</t>
-  </si>
-  <si>
-    <t>Transaction data graph</t>
-  </si>
-  <si>
-    <t>Transaction data section</t>
-  </si>
-  <si>
-    <t>Screening conditions</t>
-  </si>
-  <si>
-    <t>Business Data</t>
-  </si>
-  <si>
-    <t>Merchant Details</t>
-  </si>
-  <si>
-    <t>User Management</t>
-  </si>
-  <si>
-    <t>Level setting</t>
-  </si>
-  <si>
-    <t>Add user</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>Mute</t>
-  </si>
-  <si>
-    <t>Blacklist</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Data list</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>Level Settings</t>
-  </si>
-  <si>
-    <t>Hierarchical conditions:</t>
-  </si>
-  <si>
-    <t>Customize the level name</t>
-  </si>
-  <si>
-    <t>Union Management</t>
-  </si>
-  <si>
-    <t>Anchor Management</t>
-  </si>
-  <si>
-    <t>Permission Management</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>Role</t>
   </si>
@@ -112,12 +28,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Platform Management Configuration</t>
-  </si>
-  <si>
     <t>数据总览</t>
   </si>
   <si>
@@ -368,6 +278,18 @@
   </si>
   <si>
     <t>none exist</t>
+  </si>
+  <si>
+    <t>API protocol for all pages</t>
+  </si>
+  <si>
+    <t>Table height( when count is less than one page capacity)</t>
+  </si>
+  <si>
+    <t>Responsible(Flex)</t>
+  </si>
+  <si>
+    <t>Missing Contents</t>
   </si>
 </sst>
 </file>
@@ -407,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +372,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -465,7 +393,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -521,6 +449,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -798,198 +729,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C35"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="13"/>
-    <col min="2" max="2" width="37.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="C5" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="C6" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="C7" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="C8" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="C9" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="C10" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="C14" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="C15" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="C16" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="C17" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="C18" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="C19" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="C20" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="C21" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="C26" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="C33" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="C34" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -1008,10 +750,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1">
@@ -1019,26 +761,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1046,10 +788,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8"/>
     </row>
@@ -1058,10 +800,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1">
@@ -1069,26 +811,26 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1">
@@ -1096,10 +838,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1107,10 +849,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1">
@@ -1118,10 +860,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="12" customFormat="1">
@@ -1129,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="12" customFormat="1">
@@ -1140,10 +882,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1">
@@ -1151,10 +893,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1">
@@ -1162,10 +904,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1">
@@ -1173,10 +915,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="12" customFormat="1">
@@ -1184,10 +926,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1195,10 +937,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1206,10 +948,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1">
@@ -1217,10 +959,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1228,10 +970,10 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1">
@@ -1239,56 +981,56 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1">
       <c r="D23" s="10" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1">
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1">
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1">
       <c r="D26" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1">
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1">
@@ -1296,32 +1038,32 @@
         <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1">
       <c r="D29" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1">
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1329,16 +1071,16 @@
         <v>21</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1346,10 +1088,10 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1357,16 +1099,16 @@
         <v>22</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1374,10 +1116,10 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1385,16 +1127,16 @@
         <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1402,10 +1144,10 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1413,10 +1155,10 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1424,16 +1166,16 @@
         <v>24</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1441,37 +1183,157 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="12" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>115</v>
-      </c>
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="46.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="15"/>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="15"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed layout and adding function in editPage.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="11904" activeTab="1"/>
+    <workbookView windowWidth="21000" windowHeight="8627" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>数据总览</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>selectable text in cell to show dialog</t>
+  </si>
+  <si>
+    <t>upload image status</t>
   </si>
 </sst>
 </file>
@@ -295,10 +298,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -341,7 +344,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,30 +352,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,36 +367,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,47 +404,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -483,8 +471,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,187 +538,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,26 +726,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -777,37 +765,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -826,6 +794,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -834,145 +831,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1854,7 +1851,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1892,7 +1889,10 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="3:3">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="3:3">

</xml_diff>

<commit_message>
Added gift pages in activity vue.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8627" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9492" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
   <si>
     <t>数据总览</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>upload image status</t>
+  </si>
+  <si>
+    <t>Seperated to component</t>
   </si>
 </sst>
 </file>
@@ -1851,7 +1854,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1895,7 +1898,10 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="3:3">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="3:3">

</xml_diff>

<commit_message>
Added reward config page in wheel activity.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Ant-Vue\ZCool-live-broadcast-systemdev-\1.docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9492" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>数据总览</t>
   </si>
@@ -294,44 +299,44 @@
   </si>
   <si>
     <t>Seperated to component</t>
+  </si>
+  <si>
+    <t>Modal Dialog 'X' button action.</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1A1A1A"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -345,152 +350,8 @@
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,7 +366,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149998474074526"/>
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,188 +400,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -728,251 +409,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1038,61 +477,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1350,29 +745,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="19.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="15.2222222222222" customWidth="1"/>
-    <col min="5" max="5" width="26.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="15.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="6" customFormat="1" spans="1:3">
+    <row r="2" spans="1:5" s="6" customFormat="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1383,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="1" spans="1:5">
+    <row r="3" spans="1:5" s="6" customFormat="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1400,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="1" spans="2:5">
+    <row r="4" spans="1:5" s="6" customFormat="1">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="6" t="s">
@@ -1410,7 +805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1422,7 +817,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" s="6" customFormat="1" spans="1:3">
+    <row r="6" spans="1:5" s="6" customFormat="1">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1433,7 +828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="1" spans="1:5">
+    <row r="7" spans="1:5" s="6" customFormat="1">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1450,7 +845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" s="6" customFormat="1" spans="2:5">
+    <row r="8" spans="1:5" s="6" customFormat="1">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="6" t="s">
@@ -1460,7 +855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" s="6" customFormat="1" spans="1:3">
+    <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1471,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1482,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" s="6" customFormat="1" spans="1:3">
+    <row r="11" spans="1:5" s="6" customFormat="1">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -1493,7 +888,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="1" spans="1:3">
+    <row r="12" spans="1:5" s="7" customFormat="1">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -1504,7 +899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="1" spans="1:3">
+    <row r="13" spans="1:5" s="7" customFormat="1">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1515,7 +910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" s="7" customFormat="1" spans="1:3">
+    <row r="14" spans="1:5" s="7" customFormat="1">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -1526,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" s="8" customFormat="1" spans="1:3">
+    <row r="15" spans="1:5" s="8" customFormat="1">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -1537,7 +932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" s="8" customFormat="1" spans="1:3">
+    <row r="16" spans="1:5" s="8" customFormat="1">
       <c r="A16" s="8">
         <v>13</v>
       </c>
@@ -1548,7 +943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
+    <row r="17" spans="1:5" s="7" customFormat="1">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -1559,7 +954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1570,18 +965,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
+    <row r="19" spans="1:5" s="7" customFormat="1">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" s="6" customFormat="1" spans="1:3">
+    <row r="20" spans="1:5" s="6" customFormat="1">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -1592,7 +987,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1603,7 +998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" s="6" customFormat="1" spans="1:5">
+    <row r="22" spans="1:5" s="6" customFormat="1">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -1620,7 +1015,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="1" spans="4:5">
+    <row r="23" spans="1:5" s="6" customFormat="1">
       <c r="D23" s="17" t="s">
         <v>44</v>
       </c>
@@ -1628,7 +1023,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" s="6" customFormat="1" spans="4:5">
+    <row r="24" spans="1:5" s="6" customFormat="1">
       <c r="D24" s="6" t="s">
         <v>46</v>
       </c>
@@ -1636,7 +1031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="1" spans="4:5">
+    <row r="25" spans="1:5" s="6" customFormat="1">
       <c r="D25" s="6" t="s">
         <v>47</v>
       </c>
@@ -1644,7 +1039,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" s="6" customFormat="1" spans="4:5">
+    <row r="26" spans="1:5" s="6" customFormat="1">
       <c r="D26" s="6" t="s">
         <v>49</v>
       </c>
@@ -1652,7 +1047,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" s="6" customFormat="1" spans="4:5">
+    <row r="27" spans="1:5" s="6" customFormat="1">
       <c r="D27" s="6" t="s">
         <v>51</v>
       </c>
@@ -1660,7 +1055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" s="6" customFormat="1" spans="1:5">
+    <row r="28" spans="1:5" s="6" customFormat="1">
       <c r="A28" s="6">
         <v>20</v>
       </c>
@@ -1677,7 +1072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" s="6" customFormat="1" spans="4:5">
+    <row r="29" spans="1:5" s="6" customFormat="1">
       <c r="D29" s="6" t="s">
         <v>57</v>
       </c>
@@ -1685,7 +1080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" s="6" customFormat="1" spans="4:5">
+    <row r="30" spans="1:5" s="6" customFormat="1">
       <c r="D30" s="6" t="s">
         <v>59</v>
       </c>
@@ -1816,66 +1211,66 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:5">
       <c r="A41" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:5">
       <c r="A42" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="19"/>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:5">
       <c r="A44" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="46.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.3333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5555555555556" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="1" width="46.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1904,77 +1299,79 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:3">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="3:3">
+    <row r="10" spans="1:3">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="3:3">
+    <row r="11" spans="1:3">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="1:3">
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="1:3">
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="3:3">
+    <row r="14" spans="1:3">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="3:3">
+    <row r="15" spans="1:3">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="3:3">
+    <row r="16" spans="1:3">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="2:3">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="2:3">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="2:3">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="2:3">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="2:3">
       <c r="C21" s="3"/>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="3:3">
+    <row r="26" spans="2:3">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:3">
       <c r="B27" s="4"/>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4"/>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="2:3">
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="2:3">
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="2:3">
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:3">
       <c r="B35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added withdrawalRecord page in wheel page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
   <si>
     <t>数据总览</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Add binding data variable for every components</t>
   </si>
 </sst>
 </file>
@@ -753,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1248,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1306,6 +1309,9 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3">

</xml_diff>

<commit_message>
Added wheel popup page in index.vue.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Status" sheetId="2" r:id="rId1"/>
+    <sheet name="Have to fix" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
   <si>
     <t>数据总览</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>Add binding data variable for every components</t>
+  </si>
+  <si>
+    <t>Correct meaning key value of all components</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E45"/>
+  <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1231,14 +1234,12 @@
       <c r="A43" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="B43" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="8" t="s">
+      <c r="A44" s="8" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1251,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1315,6 +1316,9 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">

</xml_diff>

<commit_message>
Fixed GiftPanel to show image it's icon area and moved to components.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Ant-Vue\ZCool-live-broadcast-systemdev-\1.docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9492"/>
+    <workbookView windowWidth="20496" windowHeight="8064" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
   <si>
     <t>数据总览</t>
   </si>
@@ -271,6 +266,9 @@
     <t>site exist</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>both exist</t>
   </si>
   <si>
@@ -280,7 +278,7 @@
     <t>none exist</t>
   </si>
   <si>
-    <t>Missing Contents</t>
+    <t>Fixed</t>
   </si>
   <si>
     <t>API protocol for all pages</t>
@@ -304,45 +302,51 @@
     <t>Modal Dialog 'X' button action.</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Add binding data variable for every components</t>
   </si>
   <si>
     <t>Correct meaning key value of all components</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1A1A1A"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -356,8 +360,152 @@
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,7 +520,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +538,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <fgColor theme="0" tint="-0.14996795556505"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,8 +554,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -415,13 +749,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -434,6 +1010,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -483,17 +1062,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -751,216 +1374,216 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="19.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="15.2222222222222" customWidth="1"/>
+    <col min="5" max="5" width="26.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="15.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="6" customFormat="1">
-      <c r="A2" s="6">
+    <row r="2" s="7" customFormat="1" spans="1:3">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1">
-      <c r="A3" s="6">
+    <row r="3" s="7" customFormat="1" spans="1:5">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="6" t="s">
+    <row r="4" s="7" customFormat="1" spans="2:5">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1">
-      <c r="A6" s="6">
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" s="7" customFormat="1" spans="1:3">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1">
-      <c r="A7" s="6">
+    <row r="7" s="7" customFormat="1" spans="1:5">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="6" t="s">
+    <row r="8" s="7" customFormat="1" spans="2:5">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1">
-      <c r="A9" s="6">
+    <row r="9" s="7" customFormat="1" spans="1:3">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1">
-      <c r="A11" s="6">
+    <row r="11" s="7" customFormat="1" spans="1:3">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="7" customFormat="1">
-      <c r="A12" s="7">
+    <row r="12" s="8" customFormat="1" spans="1:3">
+      <c r="A12" s="8">
         <v>9</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="7" customFormat="1">
-      <c r="A13" s="7">
+    <row r="13" s="8" customFormat="1" spans="1:3">
+      <c r="A13" s="8">
         <v>10</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1">
-      <c r="A14" s="7">
+    <row r="14" s="8" customFormat="1" spans="1:3">
+      <c r="A14" s="8">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1">
-      <c r="A15" s="8">
+    <row r="15" s="9" customFormat="1" spans="1:3">
+      <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1">
-      <c r="A16" s="8">
+    <row r="16" s="9" customFormat="1" spans="1:3">
+      <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1">
-      <c r="A17" s="7">
+    <row r="17" s="8" customFormat="1" spans="1:3">
+      <c r="A17" s="8">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -971,29 +1594,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="7" customFormat="1">
-      <c r="A19" s="7">
+    <row r="19" s="8" customFormat="1" spans="1:3">
+      <c r="A19" s="8">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1">
-      <c r="A20" s="6">
+    <row r="20" s="7" customFormat="1" spans="1:3">
+      <c r="A20" s="7">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1004,308 +1627,310 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1">
-      <c r="A22" s="6">
+    <row r="22" s="7" customFormat="1" spans="1:5">
+      <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1">
-      <c r="D23" s="17" t="s">
+    <row r="23" s="7" customFormat="1" spans="4:5">
+      <c r="D23" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1">
-      <c r="D24" s="6" t="s">
+    <row r="24" s="7" customFormat="1" spans="4:5">
+      <c r="D24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1">
-      <c r="D25" s="6" t="s">
+    <row r="25" s="7" customFormat="1" spans="4:5">
+      <c r="D25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1">
-      <c r="D26" s="6" t="s">
+    <row r="26" s="7" customFormat="1" spans="4:5">
+      <c r="D26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1">
-      <c r="D27" s="6" t="s">
+    <row r="27" s="7" customFormat="1" spans="4:5">
+      <c r="D27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1">
-      <c r="A28" s="6">
+    <row r="28" s="7" customFormat="1" spans="1:5">
+      <c r="A28" s="7">
         <v>20</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1">
-      <c r="D29" s="6" t="s">
+    <row r="29" s="7" customFormat="1" spans="4:5">
+      <c r="D29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1">
-      <c r="D30" s="6" t="s">
+    <row r="30" s="7" customFormat="1" spans="4:5">
+      <c r="D30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18">
+      <c r="A31" s="19">
         <v>21</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="19" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="18">
+      <c r="A33" s="19">
         <v>22</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="18">
+      <c r="A35" s="19">
         <v>23</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18" t="s">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="18">
+      <c r="A38" s="19">
         <v>24</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18" t="s">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="13" t="s">
+    <row r="41" spans="1:1">
+      <c r="A41" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="18" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="6" t="s">
+      <c r="B42" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="7" t="s">
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="46.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.3333333333333" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5555555555556" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>90</v>
+      <c r="A5" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -1322,66 +1947,70 @@
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="4"/>
+    <row r="12" spans="2:3">
+      <c r="B12" s="5"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="4"/>
+    <row r="13" spans="2:3">
+      <c r="B13" s="5"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="3:3">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="3:3">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="3:3">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="3:3">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="3:3">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="3:3">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="3:3">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="3:3">
       <c r="C21" s="3"/>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="3:3">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="4"/>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="4"/>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="4"/>
+    <row r="27" spans="2:2">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="5"/>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added group page in user management vue using jsx script.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>数据总览</t>
   </si>
@@ -296,7 +296,7 @@
     <t>upload image status</t>
   </si>
   <si>
-    <t>Seperated to component</t>
+    <t>Seperated into each component</t>
   </si>
   <si>
     <t>Modal Dialog 'X' button action.</t>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>background panel card</t>
+  </si>
+  <si>
+    <t>Arrange and clean code structure</t>
   </si>
 </sst>
 </file>
@@ -316,10 +322,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -369,23 +375,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -407,21 +404,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,7 +435,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,44 +458,60 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,187 +562,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,11 +752,48 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -776,63 +813,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -847,6 +827,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -855,10 +855,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -867,133 +867,133 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1878,12 +1878,12 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="46.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.3333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.3333333333333" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.5555555555556" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88888888888889" style="1"/>
@@ -1952,11 +1952,17 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added livebroadcast management. Added test code of grid pagination into test.vue.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -4,18 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20496" windowHeight="8064" activeTab="1"/>
+    <workbookView windowWidth="20496" windowHeight="7895"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
     <sheet name="Have to fix" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="103">
   <si>
     <t>数据总览</t>
   </si>
@@ -29,24 +42,42 @@
     <t>User management</t>
   </si>
   <si>
+    <t>docx exist</t>
+  </si>
+  <si>
     <t>层级管理</t>
   </si>
   <si>
     <t>Hierarchy Management</t>
   </si>
   <si>
+    <t>site exist</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>账号风控管理</t>
   </si>
   <si>
     <t>Account risk control management</t>
   </si>
   <si>
+    <t>both exist</t>
+  </si>
+  <si>
+    <t>not completed</t>
+  </si>
+  <si>
     <t>工会管理</t>
   </si>
   <si>
     <t>union management</t>
   </si>
   <si>
+    <t>none exist</t>
+  </si>
+  <si>
     <t>主播管理</t>
   </si>
   <si>
@@ -122,7 +153,7 @@
     <t>活动管理</t>
   </si>
   <si>
-    <t>event management</t>
+    <t>activity management</t>
   </si>
   <si>
     <t>消息管理</t>
@@ -260,22 +291,13 @@
     <t>Marquee Configuration</t>
   </si>
   <si>
-    <t>docx exist</t>
-  </si>
-  <si>
-    <t>site exist</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>both exist</t>
-  </si>
-  <si>
-    <t>not completed</t>
-  </si>
-  <si>
-    <t>none exist</t>
+    <t>代理管理</t>
+  </si>
+  <si>
+    <t>Agent Management</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
   <si>
     <t>Fixed</t>
@@ -320,14 +342,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,29 +384,70 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="16.5"/>
+      <color rgb="FF1F2329"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,15 +459,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,29 +484,43 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -442,70 +528,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -538,6 +575,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -562,13 +605,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,163 +773,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,11 +787,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,26 +835,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -813,17 +865,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -838,166 +884,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1028,12 +1065,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1043,73 +1086,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1380,207 +1432,230 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:E44"/>
+  <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="19.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="44.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="25.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="15.2222222222222" customWidth="1"/>
     <col min="5" max="5" width="26.5555555555556" customWidth="1"/>
     <col min="6" max="6" width="15.2222222222222" customWidth="1"/>
+    <col min="7" max="7" width="11.8888888888889" customWidth="1"/>
+    <col min="8" max="8" width="15.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="7" customFormat="1" spans="1:3">
+    <row r="2" s="7" customFormat="1" spans="1:6">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" s="7" customFormat="1" spans="1:5">
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" s="7" customFormat="1" spans="1:13">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" s="7" customFormat="1" spans="2:5">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="L3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3"/>
+    </row>
+    <row r="4" s="7" customFormat="1" spans="2:13">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" s="7" customFormat="1" spans="1:3">
+      <c r="B5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="L5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" s="7" customFormat="1" spans="1:13">
       <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6"/>
     </row>
     <row r="7" s="7" customFormat="1" spans="1:5">
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>11</v>
+      <c r="B7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" s="7" customFormat="1" spans="2:5">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" s="7" customFormat="1" spans="1:3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>15</v>
+      <c r="B9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>17</v>
+      <c r="B10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="1" spans="1:3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
+      <c r="B11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" s="8" customFormat="1" spans="1:3">
       <c r="A12" s="8">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" s="8" customFormat="1" spans="1:3">
-      <c r="A13" s="8">
+      <c r="B12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" s="9" customFormat="1" spans="1:3">
+      <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" s="8" customFormat="1" spans="1:3">
-      <c r="A14" s="8">
+      <c r="B13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" s="9" customFormat="1" spans="1:3">
+      <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" s="9" customFormat="1" spans="1:3">
-      <c r="A15" s="9">
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" s="10" customFormat="1" spans="1:3">
+      <c r="A15" s="10">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" s="9" customFormat="1" spans="1:3">
-      <c r="A16" s="9">
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" s="10" customFormat="1" spans="1:3">
+      <c r="A16" s="10">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" s="8" customFormat="1" spans="1:3">
-      <c r="A17" s="8">
+      <c r="B16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" s="9" customFormat="1" spans="1:3">
+      <c r="A17" s="9">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>31</v>
+      <c r="B17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1588,21 +1663,21 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" s="8" customFormat="1" spans="1:3">
-      <c r="A19" s="8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" s="9" customFormat="1" spans="1:3">
+      <c r="A19" s="9">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>35</v>
+      <c r="B19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="1" spans="1:3">
@@ -1610,10 +1685,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1621,10 +1696,10 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" s="7" customFormat="1" spans="1:5">
@@ -1632,56 +1707,56 @@
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" s="7" customFormat="1" spans="4:5">
-      <c r="D23" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>45</v>
+      <c r="D23" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" s="7" customFormat="1" spans="4:5">
       <c r="D24" s="7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" s="7" customFormat="1" spans="4:5">
       <c r="D25" s="7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" s="7" customFormat="1" spans="4:5">
       <c r="D26" s="7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" s="7" customFormat="1" spans="4:5">
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" s="7" customFormat="1" spans="1:5">
@@ -1689,181 +1764,174 @@
         <v>20</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" s="7" customFormat="1" spans="4:5">
       <c r="D29" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" s="7" customFormat="1" spans="4:5">
       <c r="D30" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="19">
+      <c r="A31" s="23">
         <v>21</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>63</v>
+      <c r="B31" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="23">
+        <v>22</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="19">
-        <v>22</v>
-      </c>
-      <c r="B33" s="19" t="s">
+      <c r="E34" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="19">
+      <c r="A35" s="23">
         <v>23</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>71</v>
+      <c r="B35" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>73</v>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>75</v>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="19">
+      <c r="A38" s="23">
         <v>24</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>77</v>
+      <c r="B38" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>80</v>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" ht="21" spans="1:4">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="9" t="s">
-        <v>86</v>
+      <c r="A41">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1877,7 +1945,7 @@
   <sheetPr/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1891,77 +1959,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>

</xml_diff>

<commit_message>
Added sports page in live broadcast management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1009,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M65"/>
+  <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1027,7 +1027,7 @@
     <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="7" customFormat="1" ht="15.6">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="15.6">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1060,12 +1060,8 @@
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="L3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="15.6">
+    </row>
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A4" s="15"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -1077,14 +1073,8 @@
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="L4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.6">
+    </row>
+    <row r="5" spans="1:7" ht="15.6">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -1098,14 +1088,8 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="L5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="15.6">
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1119,12 +1103,8 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="L6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="15.6">
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -1143,7 +1123,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="15.6">
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A8" s="15"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -1156,7 +1136,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="15.6">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A9" s="15">
         <v>6</v>
       </c>
@@ -1171,7 +1151,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="15.6">
+    <row r="10" spans="1:7" ht="15.6">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -1186,7 +1166,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" ht="15.6">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A11" s="15">
         <v>8</v>
       </c>
@@ -1201,7 +1181,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" ht="15.6">
+    <row r="12" spans="1:7" s="8" customFormat="1" ht="15.6">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -1216,7 +1196,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:13" s="9" customFormat="1" ht="15.6">
+    <row r="13" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A13" s="19">
         <v>10</v>
       </c>
@@ -1231,7 +1211,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1" ht="15.6">
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A14" s="19">
         <v>11</v>
       </c>
@@ -1246,7 +1226,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:13" s="11" customFormat="1" ht="15.6">
+    <row r="15" spans="1:7" s="11" customFormat="1" ht="15.6">
       <c r="A15" s="17">
         <v>12</v>
       </c>
@@ -1261,7 +1241,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:13" s="10" customFormat="1" ht="15.6">
+    <row r="16" spans="1:7" s="10" customFormat="1" ht="15.6">
       <c r="A16" s="20">
         <v>13</v>
       </c>
@@ -1276,7 +1256,7 @@
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="1:11" s="9" customFormat="1" ht="15.6">
+    <row r="17" spans="1:52" s="9" customFormat="1" ht="15.6">
       <c r="A17" s="19">
         <v>14</v>
       </c>
@@ -1291,7 +1271,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:11" s="9" customFormat="1" ht="15.6">
+    <row r="18" spans="1:52" s="9" customFormat="1" ht="15.6">
       <c r="A18" s="19">
         <v>15</v>
       </c>
@@ -1306,7 +1286,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:11" s="9" customFormat="1" ht="15.6">
+    <row r="19" spans="1:52" s="9" customFormat="1" ht="15.6">
       <c r="A19" s="19">
         <v>16</v>
       </c>
@@ -1321,7 +1301,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="20" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A20" s="15">
         <v>17</v>
       </c>
@@ -1336,7 +1316,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:11" ht="15.6">
+    <row r="21" spans="1:52" ht="15.6">
       <c r="A21" s="16">
         <v>18</v>
       </c>
@@ -1351,7 +1331,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="22" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A22" s="15">
         <v>19</v>
       </c>
@@ -1370,7 +1350,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="23" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1383,7 +1363,7 @@
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
     </row>
-    <row r="24" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="24" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1396,20 +1376,20 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="25" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="26" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1422,7 +1402,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="27" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1435,7 +1415,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="28" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1448,7 +1428,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="29" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1461,7 +1441,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="30" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1474,7 +1454,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:11" s="11" customFormat="1" ht="15.6">
+    <row r="31" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1490,8 +1470,49 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" s="11" customFormat="1" ht="15.6">
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7"/>
+      <c r="AL31" s="7"/>
+      <c r="AM31" s="7"/>
+      <c r="AN31" s="7"/>
+      <c r="AO31" s="7"/>
+      <c r="AP31" s="7"/>
+      <c r="AQ31" s="7"/>
+      <c r="AR31" s="7"/>
+      <c r="AS31" s="7"/>
+      <c r="AT31" s="7"/>
+      <c r="AU31" s="7"/>
+      <c r="AV31" s="7"/>
+      <c r="AW31" s="7"/>
+      <c r="AX31" s="7"/>
+      <c r="AY31" s="7"/>
+      <c r="AZ31" s="7"/>
+    </row>
+    <row r="32" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -1507,8 +1528,49 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-    </row>
-    <row r="33" spans="1:11" s="7" customFormat="1" ht="15.6">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="7"/>
+      <c r="AL32" s="7"/>
+      <c r="AM32" s="7"/>
+      <c r="AN32" s="7"/>
+      <c r="AO32" s="7"/>
+      <c r="AP32" s="7"/>
+      <c r="AQ32" s="7"/>
+      <c r="AR32" s="7"/>
+      <c r="AS32" s="7"/>
+      <c r="AT32" s="7"/>
+      <c r="AU32" s="7"/>
+      <c r="AV32" s="7"/>
+      <c r="AW32" s="7"/>
+      <c r="AX32" s="7"/>
+      <c r="AY32" s="7"/>
+      <c r="AZ32" s="7"/>
+    </row>
+    <row r="33" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1521,7 +1583,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:11" s="11" customFormat="1" ht="15.6">
+    <row r="34" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1537,8 +1599,49 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-    </row>
-    <row r="35" spans="1:11" s="11" customFormat="1" ht="15.6">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="7"/>
+      <c r="AK34" s="7"/>
+      <c r="AL34" s="7"/>
+      <c r="AM34" s="7"/>
+      <c r="AN34" s="7"/>
+      <c r="AO34" s="7"/>
+      <c r="AP34" s="7"/>
+      <c r="AQ34" s="7"/>
+      <c r="AR34" s="7"/>
+      <c r="AS34" s="7"/>
+      <c r="AT34" s="7"/>
+      <c r="AU34" s="7"/>
+      <c r="AV34" s="7"/>
+      <c r="AW34" s="7"/>
+      <c r="AX34" s="7"/>
+      <c r="AY34" s="7"/>
+      <c r="AZ34" s="7"/>
+    </row>
+    <row r="35" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -1554,8 +1657,49 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" s="11" customFormat="1" ht="15.6">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="7"/>
+      <c r="AO35" s="7"/>
+      <c r="AP35" s="7"/>
+      <c r="AQ35" s="7"/>
+      <c r="AR35" s="7"/>
+      <c r="AS35" s="7"/>
+      <c r="AT35" s="7"/>
+      <c r="AU35" s="7"/>
+      <c r="AV35" s="7"/>
+      <c r="AW35" s="7"/>
+      <c r="AX35" s="7"/>
+      <c r="AY35" s="7"/>
+      <c r="AZ35" s="7"/>
+    </row>
+    <row r="36" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -1571,8 +1715,49 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" s="11" customFormat="1" ht="15.6">
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7"/>
+      <c r="AJ36" s="7"/>
+      <c r="AK36" s="7"/>
+      <c r="AL36" s="7"/>
+      <c r="AM36" s="7"/>
+      <c r="AN36" s="7"/>
+      <c r="AO36" s="7"/>
+      <c r="AP36" s="7"/>
+      <c r="AQ36" s="7"/>
+      <c r="AR36" s="7"/>
+      <c r="AS36" s="7"/>
+      <c r="AT36" s="7"/>
+      <c r="AU36" s="7"/>
+      <c r="AV36" s="7"/>
+      <c r="AW36" s="7"/>
+      <c r="AX36" s="7"/>
+      <c r="AY36" s="7"/>
+      <c r="AZ36" s="7"/>
+    </row>
+    <row r="37" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1588,8 +1773,49 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-    </row>
-    <row r="38" spans="1:11" s="7" customFormat="1" ht="15.6">
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
+      <c r="AL37" s="7"/>
+      <c r="AM37" s="7"/>
+      <c r="AN37" s="7"/>
+      <c r="AO37" s="7"/>
+      <c r="AP37" s="7"/>
+      <c r="AQ37" s="7"/>
+      <c r="AR37" s="7"/>
+      <c r="AS37" s="7"/>
+      <c r="AT37" s="7"/>
+      <c r="AU37" s="7"/>
+      <c r="AV37" s="7"/>
+      <c r="AW37" s="7"/>
+      <c r="AX37" s="7"/>
+      <c r="AY37" s="7"/>
+      <c r="AZ37" s="7"/>
+    </row>
+    <row r="38" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A38" s="15">
         <v>20</v>
       </c>
@@ -1608,7 +1834,7 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="39" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -1621,7 +1847,7 @@
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="7" customFormat="1" ht="15.6">
+    <row r="40" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -1634,7 +1860,7 @@
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="41" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A41" s="21">
         <v>21</v>
       </c>
@@ -1653,7 +1879,7 @@
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
     </row>
-    <row r="42" spans="1:11" s="9" customFormat="1" ht="15.6">
+    <row r="42" spans="1:52" s="9" customFormat="1" ht="15.6">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -1666,7 +1892,7 @@
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="43" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A43" s="21">
         <v>22</v>
       </c>
@@ -1685,7 +1911,7 @@
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="44" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -1698,7 +1924,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="45" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A45" s="21">
         <v>23</v>
       </c>
@@ -1717,7 +1943,7 @@
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="46" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -1730,7 +1956,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="47" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -1743,7 +1969,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="15.6">
+    <row r="48" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A48" s="21">
         <v>24</v>
       </c>
@@ -2014,6 +2240,32 @@
       <c r="E65" s="16"/>
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="B68" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="B69" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed to show placeholder and etc in all pages in activity management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -704,9 +704,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -732,6 +729,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1031,10 +1031,10 @@
       <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="15"/>
@@ -1046,16 +1046,16 @@
       <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="15"/>
@@ -1063,8 +1063,8 @@
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A4" s="15"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
@@ -1078,10 +1078,10 @@
       <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="17"/>
@@ -1093,10 +1093,10 @@
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="15"/>
@@ -1108,16 +1108,16 @@
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="15"/>
@@ -1125,8 +1125,8 @@
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A8" s="15"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="15" t="s">
         <v>17</v>
       </c>
@@ -1140,10 +1140,10 @@
       <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="15"/>
@@ -1155,10 +1155,10 @@
       <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="16"/>
@@ -1170,10 +1170,10 @@
       <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="15"/>
@@ -1185,10 +1185,10 @@
       <c r="A12" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="18"/>
@@ -1200,10 +1200,10 @@
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="19"/>
@@ -1360,8 +1360,8 @@
       <c r="E23" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A24" s="15"/>
@@ -2076,29 +2076,29 @@
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6">
-      <c r="A55" s="17">
+    <row r="55" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A55" s="19">
         <v>30</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
     </row>
     <row r="56" spans="1:7" ht="15.6">
       <c r="A56" s="17">
         <v>31</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D56" s="17"/>
@@ -2125,7 +2125,7 @@
       <c r="A58" s="17">
         <v>33</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="27" t="s">
         <v>114</v>
       </c>
       <c r="C58" s="16" t="s">
@@ -2140,7 +2140,7 @@
       <c r="A59" s="17">
         <v>34</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="24" t="s">
         <v>116</v>
       </c>
       <c r="C59" s="16" t="s">
@@ -2155,7 +2155,7 @@
       <c r="A60" s="17">
         <v>35</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="32" t="s">
         <v>118</v>
       </c>
       <c r="C60" s="16" t="s">
@@ -2185,7 +2185,7 @@
       <c r="A62" s="17">
         <v>37</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="32" t="s">
         <v>122</v>
       </c>
       <c r="C62" s="16" t="s">
@@ -2200,7 +2200,7 @@
       <c r="A63" s="17">
         <v>38</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>124</v>
       </c>
       <c r="C63" s="16" t="s">
@@ -2215,7 +2215,7 @@
       <c r="A64" s="17">
         <v>39</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="32" t="s">
         <v>111</v>
       </c>
       <c r="C64" s="16" t="s">

</xml_diff>

<commit_message>
1. 共 {{ totalItems }} 条 -> 共 {{ totalItems }}条 2. Add first deposit management page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Fixed exportList, add function of discountRecord page. Fixed reset function of game management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2031,20 +2031,20 @@
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6">
-      <c r="A52" s="17">
+    <row r="52" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A52" s="19">
         <v>27</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:7" s="14" customFormat="1" ht="15.6">
       <c r="A53" s="22">

</xml_diff>

<commit_message>
Fixed reset, form layout, bind variables in game, order management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>数据总览</t>
   </si>
   <si>
-    <t>Data overview</t>
-  </si>
-  <si>
     <t>用户管理</t>
   </si>
   <si>
@@ -492,18 +489,37 @@
   </si>
   <si>
     <t>Level configuration(category)</t>
+  </si>
+  <si>
+    <t>Fund Management</t>
+  </si>
+  <si>
+    <t>资金管理</t>
+  </si>
+  <si>
+    <t>in Statistics</t>
+  </si>
+  <si>
+    <t>Data overview(Statistics)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -631,25 +647,25 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -677,61 +693,64 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1035,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -1047,16 +1066,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>2</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>3</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -1066,10 +1085,10 @@
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>5</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>6</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -1079,10 +1098,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>10</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="16"/>
@@ -1094,10 +1113,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -1109,16 +1128,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>15</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>16</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -1128,10 +1147,10 @@
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -1141,10 +1160,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -1156,10 +1175,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -1171,10 +1190,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>24</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1186,10 +1205,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -1201,10 +1220,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>28</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -1216,10 +1235,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -1231,10 +1250,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1246,10 +1265,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>34</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1261,10 +1280,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -1276,10 +1295,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>38</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -1291,10 +1310,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -1306,10 +1325,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -1321,10 +1340,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1336,16 +1355,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -1355,10 +1374,10 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
@@ -1368,10 +1387,10 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -1381,10 +1400,10 @@
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -1394,10 +1413,10 @@
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -1407,10 +1426,10 @@
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1420,10 +1439,10 @@
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -1433,10 +1452,10 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -1446,10 +1465,10 @@
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1459,10 +1478,10 @@
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -1517,10 +1536,10 @@
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -1575,10 +1594,10 @@
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -1588,10 +1607,10 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1646,10 +1665,10 @@
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -1704,10 +1723,10 @@
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -1762,10 +1781,10 @@
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -1820,16 +1839,16 @@
         <v>20</v>
       </c>
       <c r="B38" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="E38" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -1839,10 +1858,10 @@
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -1852,10 +1871,10 @@
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
@@ -1865,16 +1884,16 @@
         <v>21</v>
       </c>
       <c r="B41" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="D41" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
@@ -1884,10 +1903,10 @@
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>64</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -1897,16 +1916,16 @@
         <v>22</v>
       </c>
       <c r="B43" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>66</v>
-      </c>
       <c r="D43" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>66</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -1916,10 +1935,10 @@
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
@@ -1929,16 +1948,16 @@
         <v>23</v>
       </c>
       <c r="B45" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="D45" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="E45" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>70</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
@@ -1948,10 +1967,10 @@
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>72</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
@@ -1961,10 +1980,10 @@
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
@@ -1974,16 +1993,16 @@
         <v>24</v>
       </c>
       <c r="B48" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>75</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>76</v>
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
@@ -1993,10 +2012,10 @@
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>79</v>
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
@@ -2006,10 +2025,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
@@ -2021,10 +2040,10 @@
         <v>26</v>
       </c>
       <c r="B51" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
@@ -2036,10 +2055,10 @@
         <v>27</v>
       </c>
       <c r="B52" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
@@ -2051,10 +2070,10 @@
         <v>28</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -2066,10 +2085,10 @@
         <v>29</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
@@ -2081,10 +2100,10 @@
         <v>30</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
@@ -2096,10 +2115,10 @@
         <v>31</v>
       </c>
       <c r="B56" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="31" t="s">
         <v>108</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>109</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
@@ -2111,12 +2130,14 @@
         <v>32</v>
       </c>
       <c r="B57" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" s="17"/>
+      <c r="D57" s="17" t="s">
+        <v>154</v>
+      </c>
       <c r="E57" s="17"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
@@ -2126,10 +2147,10 @@
         <v>33</v>
       </c>
       <c r="B58" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
@@ -2141,10 +2162,10 @@
         <v>34</v>
       </c>
       <c r="B59" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
@@ -2156,10 +2177,10 @@
         <v>35</v>
       </c>
       <c r="B60" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
@@ -2171,10 +2192,10 @@
         <v>36</v>
       </c>
       <c r="B61" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2186,10 +2207,10 @@
         <v>37</v>
       </c>
       <c r="B62" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2201,10 +2222,10 @@
         <v>38</v>
       </c>
       <c r="B63" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2216,10 +2237,10 @@
         <v>39</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2231,40 +2252,51 @@
         <v>40</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
     </row>
+    <row r="66" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A66" s="19">
+        <v>41</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
     <row r="68" spans="1:7">
       <c r="B68" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="B70" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="B71" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2291,77 +2323,77 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>

</xml_diff>

<commit_message>
Fixed show dialogs in application4release page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -389,9 +389,6 @@
     <t>靓号管理</t>
   </si>
   <si>
-    <t>Pemium Number Management</t>
-  </si>
-  <si>
     <t>房间号管理</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t>Data overview(Statistics)</t>
+  </si>
+  <si>
+    <t>Pretty Number Management</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -1358,13 +1358,13 @@
         <v>43</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -1374,10 +1374,10 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
@@ -1387,10 +1387,10 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -1403,7 +1403,7 @@
         <v>45</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -1416,7 +1416,7 @@
         <v>46</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -1426,10 +1426,10 @@
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1442,7 +1442,7 @@
         <v>47</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -1452,10 +1452,10 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -1465,10 +1465,10 @@
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1478,10 +1478,10 @@
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -1536,10 +1536,10 @@
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -1607,10 +1607,10 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1665,10 +1665,10 @@
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -1723,10 +1723,10 @@
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -1784,7 +1784,7 @@
         <v>48</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -2136,7 +2136,7 @@
         <v>112</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="16"/>
@@ -2180,7 +2180,7 @@
         <v>117</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
@@ -2192,10 +2192,10 @@
         <v>36</v>
       </c>
       <c r="B61" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2207,10 +2207,10 @@
         <v>37</v>
       </c>
       <c r="B62" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2222,10 +2222,10 @@
         <v>38</v>
       </c>
       <c r="B63" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>123</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2252,7 +2252,7 @@
         <v>40</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>58</v>
@@ -2267,10 +2267,10 @@
         <v>41</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:7">

</xml_diff>

<commit_message>
Added copy of main page in blacklist management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2142,20 +2142,20 @@
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6">
-      <c r="A58" s="17">
+    <row r="58" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A58" s="19">
         <v>33</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" ht="15.6">
       <c r="A59" s="17">

</xml_diff>

<commit_message>
Added IP address validation function. Added fetching location from IP address in accountrisk management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="157">
   <si>
     <t>数据总览</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>Pretty Number Management</t>
+  </si>
+  <si>
+    <t>input validation function</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -2309,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2385,7 +2388,7 @@
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B12" s="5"/>
@@ -2399,6 +2402,9 @@
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3">

</xml_diff>

<commit_message>
Added some functions in IP, device pages in accountrisk management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -650,7 +650,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,9 +733,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1033,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1096,20 +1093,20 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6">
-      <c r="A5" s="16">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A5" s="19">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A6" s="15">
@@ -1207,10 +1204,10 @@
       <c r="A12" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="18"/>
@@ -1222,10 +1219,10 @@
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="19"/>
@@ -2102,7 +2099,7 @@
       <c r="A55" s="19">
         <v>30</v>
       </c>
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="32" t="s">
         <v>102</v>
       </c>
       <c r="C55" s="19" t="s">
@@ -2117,10 +2114,10 @@
       <c r="A56" s="17">
         <v>31</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="30" t="s">
         <v>108</v>
       </c>
       <c r="D56" s="17"/>
@@ -2149,7 +2146,7 @@
       <c r="A58" s="19">
         <v>33</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="29" t="s">
         <v>113</v>
       </c>
       <c r="C58" s="19" t="s">
@@ -2179,7 +2176,7 @@
       <c r="A60" s="17">
         <v>35</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="31" t="s">
         <v>117</v>
       </c>
       <c r="C60" s="16" t="s">
@@ -2209,7 +2206,7 @@
       <c r="A62" s="17">
         <v>37</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="31" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="16" t="s">
@@ -2224,7 +2221,7 @@
       <c r="A63" s="17">
         <v>38</v>
       </c>
-      <c r="B63" s="32" t="s">
+      <c r="B63" s="31" t="s">
         <v>122</v>
       </c>
       <c r="C63" s="16" t="s">
@@ -2239,7 +2236,7 @@
       <c r="A64" s="17">
         <v>39</v>
       </c>
-      <c r="B64" s="32" t="s">
+      <c r="B64" s="31" t="s">
         <v>110</v>
       </c>
       <c r="C64" s="16" t="s">
@@ -2269,7 +2266,7 @@
       <c r="A66" s="19">
         <v>41</v>
       </c>
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="33" t="s">
         <v>152</v>
       </c>
       <c r="C66" s="19" t="s">
@@ -2312,7 +2309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added a page of real-name auth in accout risk management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="158">
   <si>
     <t>数据总览</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>input validation function</t>
+  </si>
+  <si>
+    <t>needn't</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,6 +638,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -650,7 +659,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -732,9 +741,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -751,6 +757,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AZ71"/>
+  <dimension ref="A2:AZ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1097,10 +1112,10 @@
       <c r="A5" s="19">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="19"/>
@@ -1170,20 +1185,20 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6">
-      <c r="A10" s="16">
+    <row r="10" spans="1:7" s="33" customFormat="1" ht="15.6">
+      <c r="A10" s="34">
         <v>7</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A11" s="15">
@@ -1204,10 +1219,10 @@
       <c r="A12" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="18"/>
@@ -1219,10 +1234,10 @@
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="19"/>
@@ -2099,7 +2114,7 @@
       <c r="A55" s="19">
         <v>30</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="31" t="s">
         <v>102</v>
       </c>
       <c r="C55" s="19" t="s">
@@ -2114,10 +2129,10 @@
       <c r="A56" s="17">
         <v>31</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="29" t="s">
         <v>108</v>
       </c>
       <c r="D56" s="17"/>
@@ -2146,7 +2161,7 @@
       <c r="A58" s="19">
         <v>33</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="28" t="s">
         <v>113</v>
       </c>
       <c r="C58" s="19" t="s">
@@ -2176,7 +2191,7 @@
       <c r="A60" s="17">
         <v>35</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="30" t="s">
         <v>117</v>
       </c>
       <c r="C60" s="16" t="s">
@@ -2187,26 +2202,26 @@
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6">
-      <c r="A61" s="17">
+    <row r="61" spans="1:7" s="33" customFormat="1" ht="15.6">
+      <c r="A61" s="34">
         <v>36</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" spans="1:7" ht="15.6">
       <c r="A62" s="17">
         <v>37</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="30" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="16" t="s">
@@ -2221,7 +2236,7 @@
       <c r="A63" s="17">
         <v>38</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="30" t="s">
         <v>122</v>
       </c>
       <c r="C63" s="16" t="s">
@@ -2236,7 +2251,7 @@
       <c r="A64" s="17">
         <v>39</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="30" t="s">
         <v>110</v>
       </c>
       <c r="C64" s="16" t="s">
@@ -2266,7 +2281,7 @@
       <c r="A66" s="19">
         <v>41</v>
       </c>
-      <c r="B66" s="33" t="s">
+      <c r="B66" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C66" s="19" t="s">
@@ -2297,6 +2312,11 @@
     <row r="71" spans="1:7">
       <c r="B71" s="10" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="B72" s="33" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added user page in report management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
   <si>
     <t>数据总览</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>needn't</t>
+  </si>
+  <si>
+    <t>multiple select layout in a-form-create problem</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2329,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2425,6 +2428,9 @@
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3">

</xml_diff>

<commit_message>
Added commision management page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ72"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1353,20 +1353,20 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:52" ht="15.6">
-      <c r="A21" s="16">
+    <row r="21" spans="1:52" s="9" customFormat="1" ht="15.6">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A22" s="15">
@@ -2332,7 +2332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed mistakes like column width, edit dialog, ... in activity, order, strategy, blacklist managements.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
   <si>
     <t>数据总览</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>multiple select layout in a-form-create problem</t>
+  </si>
+  <si>
+    <t>星级扫描</t>
+  </si>
+  <si>
+    <t>Star Scan</t>
+  </si>
+  <si>
+    <t>分组管理</t>
+  </si>
+  <si>
+    <t>Group management</t>
   </si>
 </sst>
 </file>
@@ -750,26 +762,26 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1046,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AZ72"/>
+  <dimension ref="A2:AZ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1112,523 +1124,478 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A5" s="19">
-        <v>3</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>162</v>
+      </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A6" s="15">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A6" s="19"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A7" s="19">
+        <v>3</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A8" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A8" s="15"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A9" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" s="33" customFormat="1" ht="15.6">
-      <c r="A10" s="34">
-        <v>7</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A10" s="15"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A11" s="15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="15.6">
-      <c r="A12" s="18">
+    <row r="12" spans="1:7" s="32" customFormat="1" ht="15.6">
+      <c r="A12" s="33">
+        <v>7</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A13" s="15">
+        <v>8</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" s="8" customFormat="1" ht="15.6">
+      <c r="A14" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C14" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A13" s="19">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A15" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B15" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A14" s="19">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A16" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A15" s="17">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A17" s="17">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" s="10" customFormat="1" ht="15.6">
-      <c r="A16" s="20">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="15.6">
+      <c r="A18" s="20">
         <v>13</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B18" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A17" s="19">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A19" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B19" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A18" s="19">
-        <v>15</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A19" s="19">
-        <v>16</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A20" s="15">
-        <v>17</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:52" s="9" customFormat="1" ht="15.6">
+    <row r="20" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A20" s="19">
+        <v>15</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A21" s="19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="22" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A22" s="15">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>150</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>136</v>
+    <row r="23" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A23" s="19">
+        <v>18</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A24" s="15">
+        <v>19</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="1:52" s="7" customFormat="1" ht="15.6">
+      <c r="D25" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+    </row>
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>138</v>
+      <c r="D26" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>136</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>139</v>
+      <c r="D27" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
-      <c r="D30" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>142</v>
+      <c r="D30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="31" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
-      <c r="D31" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>143</v>
+      <c r="D31" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="7"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="7"/>
-      <c r="AQ31" s="7"/>
-      <c r="AR31" s="7"/>
-      <c r="AS31" s="7"/>
-      <c r="AT31" s="7"/>
-      <c r="AU31" s="7"/>
-      <c r="AV31" s="7"/>
-      <c r="AW31" s="7"/>
-      <c r="AX31" s="7"/>
-      <c r="AY31" s="7"/>
-      <c r="AZ31" s="7"/>
-    </row>
-    <row r="32" spans="1:52" s="11" customFormat="1" ht="15.6">
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
-      <c r="D32" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>144</v>
+      <c r="D32" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="7"/>
-      <c r="AH32" s="7"/>
-      <c r="AI32" s="7"/>
-      <c r="AJ32" s="7"/>
-      <c r="AK32" s="7"/>
-      <c r="AL32" s="7"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="7"/>
-      <c r="AO32" s="7"/>
-      <c r="AP32" s="7"/>
-      <c r="AQ32" s="7"/>
-      <c r="AR32" s="7"/>
-      <c r="AS32" s="7"/>
-      <c r="AT32" s="7"/>
-      <c r="AU32" s="7"/>
-      <c r="AV32" s="7"/>
-      <c r="AW32" s="7"/>
-      <c r="AX32" s="7"/>
-      <c r="AY32" s="7"/>
-      <c r="AZ32" s="7"/>
-    </row>
-    <row r="33" spans="1:52" s="7" customFormat="1" ht="15.6">
+    </row>
+    <row r="33" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
-      <c r="D33" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>50</v>
+      <c r="D33" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7"/>
+      <c r="AL33" s="7"/>
+      <c r="AM33" s="7"/>
+      <c r="AN33" s="7"/>
+      <c r="AO33" s="7"/>
+      <c r="AP33" s="7"/>
+      <c r="AQ33" s="7"/>
+      <c r="AR33" s="7"/>
+      <c r="AS33" s="7"/>
+      <c r="AT33" s="7"/>
+      <c r="AU33" s="7"/>
+      <c r="AV33" s="7"/>
+      <c r="AW33" s="7"/>
+      <c r="AX33" s="7"/>
+      <c r="AY33" s="7"/>
+      <c r="AZ33" s="7"/>
     </row>
     <row r="34" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1678,73 +1645,28 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="7"/>
     </row>
-    <row r="35" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="35" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
-      <c r="D35" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>146</v>
+      <c r="D35" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="7"/>
-      <c r="V35" s="7"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="7"/>
-      <c r="Y35" s="7"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="7"/>
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
-      <c r="AE35" s="7"/>
-      <c r="AF35" s="7"/>
-      <c r="AG35" s="7"/>
-      <c r="AH35" s="7"/>
-      <c r="AI35" s="7"/>
-      <c r="AJ35" s="7"/>
-      <c r="AK35" s="7"/>
-      <c r="AL35" s="7"/>
-      <c r="AM35" s="7"/>
-      <c r="AN35" s="7"/>
-      <c r="AO35" s="7"/>
-      <c r="AP35" s="7"/>
-      <c r="AQ35" s="7"/>
-      <c r="AR35" s="7"/>
-      <c r="AS35" s="7"/>
-      <c r="AT35" s="7"/>
-      <c r="AU35" s="7"/>
-      <c r="AV35" s="7"/>
-      <c r="AW35" s="7"/>
-      <c r="AX35" s="7"/>
-      <c r="AY35" s="7"/>
-      <c r="AZ35" s="7"/>
     </row>
     <row r="36" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -1798,11 +1720,11 @@
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
-      <c r="D37" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>148</v>
+      <c r="D37" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -1852,130 +1774,214 @@
       <c r="AY37" s="7"/>
       <c r="AZ37" s="7"/>
     </row>
-    <row r="38" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A38" s="15">
-        <v>20</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>54</v>
+    <row r="38" spans="1:52" s="11" customFormat="1" ht="15.6">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:52" s="7" customFormat="1" ht="15.6">
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
+      <c r="AN38" s="7"/>
+      <c r="AO38" s="7"/>
+      <c r="AP38" s="7"/>
+      <c r="AQ38" s="7"/>
+      <c r="AR38" s="7"/>
+      <c r="AS38" s="7"/>
+      <c r="AT38" s="7"/>
+      <c r="AU38" s="7"/>
+      <c r="AV38" s="7"/>
+      <c r="AW38" s="7"/>
+      <c r="AX38" s="7"/>
+      <c r="AY38" s="7"/>
+      <c r="AZ38" s="7"/>
+    </row>
+    <row r="39" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>56</v>
+        <v>148</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7"/>
+      <c r="AL39" s="7"/>
+      <c r="AM39" s="7"/>
+      <c r="AN39" s="7"/>
+      <c r="AO39" s="7"/>
+      <c r="AP39" s="7"/>
+      <c r="AQ39" s="7"/>
+      <c r="AR39" s="7"/>
+      <c r="AS39" s="7"/>
+      <c r="AT39" s="7"/>
+      <c r="AU39" s="7"/>
+      <c r="AV39" s="7"/>
+      <c r="AW39" s="7"/>
+      <c r="AX39" s="7"/>
+      <c r="AY39" s="7"/>
+      <c r="AZ39" s="7"/>
     </row>
     <row r="40" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="15">
+        <v>20</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="D40" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A41" s="21">
-        <v>21</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+    <row r="41" spans="1:52" s="7" customFormat="1" ht="15.6">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="1:52" s="7" customFormat="1" ht="15.6">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
     </row>
     <row r="43" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A43" s="21">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:52" s="12" customFormat="1" ht="15.6">
+    <row r="44" spans="1:52" s="9" customFormat="1" ht="15.6">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+        <v>62</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="1:52" s="12" customFormat="1" ht="15.6">
       <c r="A45" s="21">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
@@ -1985,42 +1991,42 @@
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
     </row>
     <row r="47" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
+      <c r="A47" s="21">
+        <v>23</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="D47" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
     <row r="48" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A48" s="21">
-        <v>24</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>105</v>
-      </c>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
@@ -2030,145 +2036,145 @@
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
     </row>
-    <row r="50" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A50" s="22">
+    <row r="50" spans="1:7" s="12" customFormat="1" ht="15.6">
+      <c r="A50" s="21">
+        <v>24</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="1:7" s="12" customFormat="1" ht="15.6">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="1:7" s="14" customFormat="1" ht="15.6">
+      <c r="A52" s="22">
         <v>25</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B52" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C52" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A51" s="19">
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+    </row>
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A53" s="19">
         <v>26</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B53" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-    </row>
-    <row r="52" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A52" s="19">
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+    </row>
+    <row r="54" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A54" s="19">
         <v>27</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B54" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A53" s="22">
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+    </row>
+    <row r="55" spans="1:7" s="14" customFormat="1" ht="15.6">
+      <c r="A55" s="22">
         <v>28</v>
       </c>
-      <c r="B53" s="23" t="s">
+      <c r="B55" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C55" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A54" s="22">
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" spans="1:7" s="14" customFormat="1" ht="15.6">
+      <c r="A56" s="22">
         <v>29</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B56" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C56" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A55" s="19">
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A57" s="19">
         <v>30</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B57" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C57" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.6">
-      <c r="A56" s="17">
-        <v>31</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C56" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.6">
-      <c r="A57" s="17">
-        <v>32</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A58" s="19">
-        <v>33</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>114</v>
+        <v>31</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>108</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="19"/>
@@ -2177,88 +2183,90 @@
     </row>
     <row r="59" spans="1:7" ht="15.6">
       <c r="A59" s="17">
-        <v>34</v>
-      </c>
-      <c r="B59" s="24" t="s">
-        <v>115</v>
+        <v>32</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="17"/>
+        <v>112</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="E59" s="17"/>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6">
-      <c r="A60" s="17">
-        <v>35</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-    </row>
-    <row r="61" spans="1:7" s="33" customFormat="1" ht="15.6">
-      <c r="A61" s="34">
-        <v>36</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
+    <row r="60" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A60" s="19">
+        <v>33</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.6">
+      <c r="A61" s="17">
+        <v>34</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
     </row>
     <row r="62" spans="1:7" ht="15.6">
       <c r="A62" s="17">
-        <v>37</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>120</v>
+        <v>35</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+        <v>155</v>
+      </c>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6">
-      <c r="A63" s="17">
-        <v>38</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+    <row r="63" spans="1:7" s="32" customFormat="1" ht="15.6">
+      <c r="A63" s="33">
+        <v>36</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
     </row>
     <row r="64" spans="1:7" ht="15.6">
       <c r="A64" s="17">
-        <v>39</v>
-      </c>
-      <c r="B64" s="30" t="s">
-        <v>110</v>
+        <v>37</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2267,58 +2275,88 @@
     </row>
     <row r="65" spans="1:7" ht="15.6">
       <c r="A65" s="17">
-        <v>40</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>124</v>
+        <v>38</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>122</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
     </row>
-    <row r="66" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A66" s="19">
+    <row r="66" spans="1:7" ht="15.6">
+      <c r="A66" s="17">
+        <v>39</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.6">
+      <c r="A67" s="17">
+        <v>40</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+    </row>
+    <row r="68" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A68" s="19">
         <v>41</v>
       </c>
-      <c r="B66" s="32" t="s">
+      <c r="B68" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C68" s="19" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
-      <c r="B68" s="11" t="s">
+    <row r="70" spans="1:7">
+      <c r="B70" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
-      <c r="B69" s="12" t="s">
+    <row r="71" spans="1:7">
+      <c r="B71" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C71" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="B70" s="7" t="s">
+    <row r="72" spans="1:7">
+      <c r="B72" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C72" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="B71" s="10" t="s">
+    <row r="73" spans="1:7">
+      <c r="B73" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="B72" s="33" t="s">
+    <row r="74" spans="1:7">
+      <c r="B74" s="32" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added agent management initial part with first page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -674,7 +674,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,9 +768,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -780,8 +777,20 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AZ74"/>
+  <dimension ref="A2:AZ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1123,31 +1132,31 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A5" s="19"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="19" t="s">
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A6" s="19"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="19" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A7" s="19">
@@ -1226,20 +1235,20 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" s="32" customFormat="1" ht="15.6">
-      <c r="A12" s="33">
+    <row r="12" spans="1:7" s="31" customFormat="1" ht="15.6">
+      <c r="A12" s="32">
         <v>7</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A13" s="15">
@@ -1271,195 +1280,191 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A15" s="19">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A15" s="34">
         <v>10</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A16" s="19">
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A17" s="19">
         <v>11</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="17" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A17" s="17">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A18" s="17">
         <v>12</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="15.6">
-      <c r="A18" s="20">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="15.6">
+      <c r="A19" s="20">
         <v>13</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C19" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A19" s="19">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A20" s="34">
         <v>14</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C20" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A20" s="19">
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A21" s="34">
         <v>15</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B21" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C21" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A21" s="19">
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A22" s="34">
         <v>16</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B22" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C22" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A22" s="15">
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A23" s="15">
         <v>17</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A23" s="19">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A24" s="34">
         <v>18</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B24" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C24" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A24" s="15">
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+    </row>
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="A25" s="15">
         <v>19</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+        <v>135</v>
+      </c>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>137</v>
+      <c r="D27" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>136</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1468,11 +1473,11 @@
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>138</v>
+      <c r="D28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -1481,11 +1486,11 @@
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>139</v>
+      <c r="D29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -1494,11 +1499,11 @@
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
-      <c r="D30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>140</v>
+      <c r="D30" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1507,11 +1512,11 @@
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
-      <c r="D31" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>141</v>
+      <c r="D31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -1521,81 +1526,36 @@
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
     </row>
-    <row r="33" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="33" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
-      <c r="D33" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>143</v>
+      <c r="D33" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
-      <c r="AE33" s="7"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="7"/>
-      <c r="AH33" s="7"/>
-      <c r="AI33" s="7"/>
-      <c r="AJ33" s="7"/>
-      <c r="AK33" s="7"/>
-      <c r="AL33" s="7"/>
-      <c r="AM33" s="7"/>
-      <c r="AN33" s="7"/>
-      <c r="AO33" s="7"/>
-      <c r="AP33" s="7"/>
-      <c r="AQ33" s="7"/>
-      <c r="AR33" s="7"/>
-      <c r="AS33" s="7"/>
-      <c r="AT33" s="7"/>
-      <c r="AU33" s="7"/>
-      <c r="AV33" s="7"/>
-      <c r="AW33" s="7"/>
-      <c r="AX33" s="7"/>
-      <c r="AY33" s="7"/>
-      <c r="AZ33" s="7"/>
     </row>
     <row r="34" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1645,86 +1605,86 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="7"/>
     </row>
-    <row r="35" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="35" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
-      <c r="D35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>50</v>
+      <c r="D35" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:52" s="11" customFormat="1" ht="15.6">
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="7"/>
+      <c r="AO35" s="7"/>
+      <c r="AP35" s="7"/>
+      <c r="AQ35" s="7"/>
+      <c r="AR35" s="7"/>
+      <c r="AS35" s="7"/>
+      <c r="AT35" s="7"/>
+      <c r="AU35" s="7"/>
+      <c r="AV35" s="7"/>
+      <c r="AW35" s="7"/>
+      <c r="AX35" s="7"/>
+      <c r="AY35" s="7"/>
+      <c r="AZ35" s="7"/>
+    </row>
+    <row r="36" spans="1:52" s="7" customFormat="1" ht="15.6">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>145</v>
+      <c r="D36" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="7"/>
-      <c r="W36" s="7"/>
-      <c r="X36" s="7"/>
-      <c r="Y36" s="7"/>
-      <c r="Z36" s="7"/>
-      <c r="AA36" s="7"/>
-      <c r="AB36" s="7"/>
-      <c r="AC36" s="7"/>
-      <c r="AD36" s="7"/>
-      <c r="AE36" s="7"/>
-      <c r="AF36" s="7"/>
-      <c r="AG36" s="7"/>
-      <c r="AH36" s="7"/>
-      <c r="AI36" s="7"/>
-      <c r="AJ36" s="7"/>
-      <c r="AK36" s="7"/>
-      <c r="AL36" s="7"/>
-      <c r="AM36" s="7"/>
-      <c r="AN36" s="7"/>
-      <c r="AO36" s="7"/>
-      <c r="AP36" s="7"/>
-      <c r="AQ36" s="7"/>
-      <c r="AR36" s="7"/>
-      <c r="AS36" s="7"/>
-      <c r="AT36" s="7"/>
-      <c r="AU36" s="7"/>
-      <c r="AV36" s="7"/>
-      <c r="AW36" s="7"/>
-      <c r="AX36" s="7"/>
-      <c r="AY36" s="7"/>
-      <c r="AZ36" s="7"/>
     </row>
     <row r="37" spans="1:52" s="11" customFormat="1" ht="15.6">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -1779,10 +1739,10 @@
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -1836,11 +1796,11 @@
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
-      <c r="D39" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>148</v>
+      <c r="D39" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -1890,34 +1850,79 @@
       <c r="AY39" s="7"/>
       <c r="AZ39" s="7"/>
     </row>
-    <row r="40" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A40" s="15">
-        <v>20</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>52</v>
-      </c>
+    <row r="40" spans="1:52" s="11" customFormat="1" ht="15.6">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="7"/>
+      <c r="AB40" s="7"/>
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7"/>
+      <c r="AE40" s="7"/>
+      <c r="AF40" s="7"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
+      <c r="AJ40" s="7"/>
+      <c r="AK40" s="7"/>
+      <c r="AL40" s="7"/>
+      <c r="AM40" s="7"/>
+      <c r="AN40" s="7"/>
+      <c r="AO40" s="7"/>
+      <c r="AP40" s="7"/>
+      <c r="AQ40" s="7"/>
+      <c r="AR40" s="7"/>
+      <c r="AS40" s="7"/>
+      <c r="AT40" s="7"/>
+      <c r="AU40" s="7"/>
+      <c r="AV40" s="7"/>
+      <c r="AW40" s="7"/>
+      <c r="AX40" s="7"/>
+      <c r="AY40" s="7"/>
+      <c r="AZ40" s="7"/>
     </row>
     <row r="41" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
+      <c r="A41" s="15">
+        <v>20</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="D41" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
@@ -1927,106 +1932,106 @@
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
     </row>
-    <row r="43" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A43" s="21">
+    <row r="43" spans="1:52" s="7" customFormat="1" ht="15.6">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="1:52" s="12" customFormat="1" ht="15.6">
+      <c r="A44" s="21">
         <v>21</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B44" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C44" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D44" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E44" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21" t="s">
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="1:52" s="9" customFormat="1" ht="15.6">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E45" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="45" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A45" s="21">
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="1:52" s="12" customFormat="1" ht="15.6">
+      <c r="A46" s="21">
         <v>22</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B46" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C46" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D46" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="E46" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>58</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
     </row>
     <row r="47" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A47" s="21">
-        <v>23</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
     <row r="48" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
+      <c r="A48" s="21">
+        <v>23</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="D48" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
@@ -2036,252 +2041,250 @@
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
     </row>
     <row r="50" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A50" s="21">
-        <v>24</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>105</v>
-      </c>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
     </row>
     <row r="51" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="21">
+        <v>24</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="D51" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
     </row>
-    <row r="52" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A52" s="22">
-        <v>25</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
+    <row r="52" spans="1:7" s="12" customFormat="1" ht="15.6">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A53" s="19">
-        <v>26</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>95</v>
+        <v>25</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>79</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
     </row>
-    <row r="54" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A54" s="19">
+    <row r="54" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A54" s="34">
+        <v>26</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+    </row>
+    <row r="55" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A55" s="34">
         <v>27</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B55" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C55" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-    </row>
-    <row r="55" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A55" s="22">
-        <v>28</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
     </row>
     <row r="56" spans="1:7" s="14" customFormat="1" ht="15.6">
       <c r="A56" s="22">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
     </row>
-    <row r="57" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A57" s="19">
+    <row r="57" spans="1:7" s="14" customFormat="1" ht="15.6">
+      <c r="A57" s="22">
+        <v>29</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+    </row>
+    <row r="58" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A58" s="34">
         <v>30</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B58" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C58" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-    </row>
-    <row r="58" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A58" s="19">
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+    </row>
+    <row r="59" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A59" s="34">
         <v>31</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B59" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C59" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.6">
-      <c r="A59" s="17">
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.6">
+      <c r="A60" s="17">
         <v>32</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B60" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C60" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D60" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-    </row>
-    <row r="60" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A60" s="19">
+      <c r="E60" s="17"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+    </row>
+    <row r="61" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A61" s="34">
         <v>33</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B61" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C61" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.6">
-      <c r="A61" s="17">
-        <v>34</v>
-      </c>
-      <c r="B61" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" spans="1:7" ht="15.6">
       <c r="A62" s="17">
-        <v>35</v>
-      </c>
-      <c r="B62" s="29" t="s">
-        <v>117</v>
+        <v>34</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
     </row>
-    <row r="63" spans="1:7" s="32" customFormat="1" ht="15.6">
-      <c r="A63" s="33">
+    <row r="63" spans="1:7" ht="15.6">
+      <c r="A63" s="17">
+        <v>35</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+    </row>
+    <row r="64" spans="1:7" s="31" customFormat="1" ht="15.6">
+      <c r="A64" s="32">
         <v>36</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B64" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="33" t="s">
+      <c r="C64" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.6">
-      <c r="A64" s="17">
-        <v>37</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
     </row>
     <row r="65" spans="1:7" ht="15.6">
       <c r="A65" s="17">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2290,13 +2293,13 @@
     </row>
     <row r="66" spans="1:7" ht="15.6">
       <c r="A66" s="17">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2305,58 +2308,73 @@
     </row>
     <row r="67" spans="1:7" ht="15.6">
       <c r="A67" s="17">
-        <v>40</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>124</v>
+        <v>39</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>110</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
       <c r="F67" s="16"/>
       <c r="G67" s="16"/>
     </row>
-    <row r="68" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A68" s="19">
+    <row r="68" spans="1:7" ht="15.6">
+      <c r="A68" s="17">
+        <v>40</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+    </row>
+    <row r="69" spans="1:7" s="13" customFormat="1" ht="15.6">
+      <c r="A69" s="34">
         <v>41</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B69" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C69" s="34" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="B70" s="11" t="s">
+    <row r="71" spans="1:7">
+      <c r="B71" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="B71" s="12" t="s">
+    <row r="72" spans="1:7">
+      <c r="B72" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C72" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="B72" s="7" t="s">
+    <row r="73" spans="1:7">
+      <c r="B73" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="B73" s="10" t="s">
+    <row r="74" spans="1:7">
+      <c r="B74" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="B74" s="32" t="s">
+    <row r="75" spans="1:7">
+      <c r="B75" s="31" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2371,7 +2389,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added initial online customer service config page. Changed some in anchor withdrawal page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
   <si>
     <t>数据总览</t>
   </si>
@@ -522,6 +522,9 @@
   </si>
   <si>
     <t>Group management</t>
+  </si>
+  <si>
+    <t>a-datetime or a-rangepicker value pass string in table data vice vera</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,12 +652,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -674,7 +671,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -717,9 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -735,16 +729,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -768,13 +753,13 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -790,6 +775,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1069,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1086,479 +1074,479 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A2" s="15">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A4" s="15"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="34" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="34" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>3</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>4</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>5</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A10" s="15"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="15" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>6</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" s="31" customFormat="1" ht="15.6">
-      <c r="A12" s="32">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" s="27" customFormat="1" ht="15.6">
+      <c r="A12" s="28">
         <v>7</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>8</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" ht="15.6">
-      <c r="A14" s="18">
+      <c r="A14" s="17">
         <v>9</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A15" s="34">
+      <c r="A15" s="30">
         <v>10</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>11</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>12</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="15.6">
-      <c r="A19" s="20">
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A19" s="16">
         <v>13</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A20" s="34">
+      <c r="A20" s="30">
         <v>14</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A21" s="34">
+      <c r="A21" s="30">
         <v>15</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A22" s="34">
+      <c r="A22" s="30">
         <v>16</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>17</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A24" s="34">
+      <c r="A24" s="30">
         <v>18</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>19</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1" ht="15.6">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16" t="s">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="17" t="s">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
@@ -1606,17 +1594,17 @@
       <c r="AZ34" s="7"/>
     </row>
     <row r="35" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="17" t="s">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -1664,30 +1652,30 @@
       <c r="AZ35" s="7"/>
     </row>
     <row r="36" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="17" t="s">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -1735,17 +1723,17 @@
       <c r="AZ37" s="7"/>
     </row>
     <row r="38" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="17" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
@@ -1793,17 +1781,17 @@
       <c r="AZ38" s="7"/>
     </row>
     <row r="39" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="17" t="s">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
@@ -1851,17 +1839,17 @@
       <c r="AZ39" s="7"/>
     </row>
     <row r="40" spans="1:52" s="11" customFormat="1" ht="15.6">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15" t="s">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
@@ -1909,441 +1897,441 @@
       <c r="AZ40" s="7"/>
     </row>
     <row r="41" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A41" s="15">
+      <c r="A41" s="14">
         <v>20</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="s">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:52" s="7" customFormat="1" ht="15.6">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A44" s="21">
+      <c r="A44" s="19">
         <v>21</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="1:52" s="9" customFormat="1" ht="15.6">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21" t="s">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A46" s="21">
+      <c r="A46" s="19">
         <v>22</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
     </row>
     <row r="47" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21" t="s">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
     </row>
     <row r="48" spans="1:52" s="12" customFormat="1" ht="15.6">
-      <c r="A48" s="21">
+      <c r="A48" s="19">
         <v>23</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21" t="s">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E49" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A51" s="21">
+      <c r="A51" s="19">
         <v>24</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="D51" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:7" s="12" customFormat="1" ht="15.6">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21" t="s">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="E52" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:7" s="9" customFormat="1" ht="15.6">
-      <c r="A53" s="19">
+      <c r="A53" s="18">
         <v>25</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A54" s="34">
+      <c r="A54" s="30">
         <v>26</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
     </row>
     <row r="55" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A55" s="34">
+      <c r="A55" s="30">
         <v>27</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="34" t="s">
+      <c r="C55" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-    </row>
-    <row r="56" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A56" s="22">
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+    </row>
+    <row r="56" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A56" s="16">
         <v>28</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="1:7" s="14" customFormat="1" ht="15.6">
-      <c r="A57" s="22">
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+    </row>
+    <row r="57" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A57" s="16">
         <v>29</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
     </row>
     <row r="58" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A58" s="34">
+      <c r="A58" s="30">
         <v>30</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
     </row>
     <row r="59" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A59" s="34">
+      <c r="A59" s="30">
         <v>31</v>
       </c>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C59" s="37" t="s">
+      <c r="C59" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
     </row>
     <row r="60" spans="1:7" ht="15.6">
-      <c r="A60" s="17">
+      <c r="A60" s="16">
         <v>32</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A61" s="34">
+      <c r="A61" s="30">
         <v>33</v>
       </c>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
     </row>
     <row r="62" spans="1:7" ht="15.6">
-      <c r="A62" s="17">
+      <c r="A62" s="16">
         <v>34</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
     </row>
     <row r="63" spans="1:7" ht="15.6">
-      <c r="A63" s="17">
+      <c r="A63" s="16">
         <v>35</v>
       </c>
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-    </row>
-    <row r="64" spans="1:7" s="31" customFormat="1" ht="15.6">
-      <c r="A64" s="32">
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+    </row>
+    <row r="64" spans="1:7" s="27" customFormat="1" ht="15.6">
+      <c r="A64" s="28">
         <v>36</v>
       </c>
-      <c r="B64" s="32" t="s">
+      <c r="B64" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
     </row>
     <row r="65" spans="1:7" ht="15.6">
-      <c r="A65" s="17">
+      <c r="A65" s="16">
         <v>37</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
     </row>
     <row r="66" spans="1:7" ht="15.6">
-      <c r="A66" s="17">
+      <c r="A66" s="16">
         <v>38</v>
       </c>
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
     </row>
     <row r="67" spans="1:7" ht="15.6">
-      <c r="A67" s="17">
+      <c r="A67" s="16">
         <v>39</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
     </row>
     <row r="68" spans="1:7" ht="15.6">
-      <c r="A68" s="17">
+      <c r="A68" s="16">
         <v>40</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A69" s="34">
+      <c r="A69" s="30">
         <v>41</v>
       </c>
-      <c r="B69" s="38" t="s">
+      <c r="B69" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="34" t="s">
+      <c r="C69" s="30" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2374,7 +2362,7 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="B75" s="31" t="s">
+      <c r="B75" s="27" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2389,12 +2377,12 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
@@ -2490,6 +2478,9 @@
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="2:3">

</xml_diff>

<commit_message>
Added some into each card of online customer config page. Fixed user, anchor withdrawal page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
   <si>
     <t>数据总览</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>a-datetime or a-rangepicker value pass string in table data vice vera</t>
+  </si>
+  <si>
+    <t>use searchParams between components and table</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2376,8 +2379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2483,35 +2486,38 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="1:3">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="1:3">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="1:3">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="1:3">
       <c r="C21" s="3"/>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="1:3">
       <c r="B25" s="5"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="1:3">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="1:3">
       <c r="B27" s="5"/>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="1:3">
       <c r="B29" s="5"/>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="1:3">
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="2:3">

</xml_diff>

<commit_message>
Added checkbox first row in IPrestrict page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="166">
   <si>
     <t>数据总览</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>use searchParams between components and table</t>
+  </si>
+  <si>
+    <t>input, input-number, password, phone, email …</t>
   </si>
 </sst>
 </file>
@@ -2380,7 +2383,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2493,6 +2496,9 @@
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3">

</xml_diff>

<commit_message>
Added marquee page in website management. Added link item in editPage of recharge activity.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2383,7 +2383,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2434,7 +2434,7 @@
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C8" s="3"/>

</xml_diff>

<commit_message>
Fixed review pages in withdrawal management.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="167">
   <si>
     <t>数据总览</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>input, input-number, password, phone, email …</t>
+  </si>
+  <si>
+    <t>required field</t>
   </si>
 </sst>
 </file>
@@ -2383,7 +2386,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2502,6 +2505,9 @@
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3">

</xml_diff>

<commit_message>
import { message } from 'ant-design-vue'
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -680,7 +680,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -784,9 +784,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1066,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ75"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2136,35 +2133,35 @@
       <c r="F55" s="30"/>
       <c r="G55" s="30"/>
     </row>
-    <row r="56" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A56" s="16">
+    <row r="56" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A56" s="18">
         <v>28</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-    </row>
-    <row r="57" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A57" s="16">
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A57" s="18">
         <v>29</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" s="13" customFormat="1" ht="15.6">
       <c r="A58" s="30">
@@ -2385,7 +2382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Showed existing management pages.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1064,7 +1064,7 @@
   <dimension ref="A2:AZ75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1328,20 +1328,20 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A19" s="16">
+    <row r="19" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A19" s="18">
         <v>13</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6">
       <c r="A20" s="30">

</xml_diff>

<commit_message>
Fixed Research/Reset buttons into group. Added binding management page. And used merchSelectRule instead of manual rule.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="169">
   <si>
     <t>数据总览</t>
   </si>
@@ -534,18 +534,31 @@
   </si>
   <si>
     <t>required field</t>
+  </si>
+  <si>
+    <t>绑定管理</t>
+  </si>
+  <si>
+    <t>Binding Management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -602,6 +615,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -680,25 +699,25 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -723,67 +742,73 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1061,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AZ75"/>
+  <dimension ref="A2:AZ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1127,30 +1152,30 @@
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="30" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="30" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A7" s="18">
@@ -1229,20 +1254,20 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" s="27" customFormat="1" ht="15.6">
-      <c r="A12" s="28">
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="15.6">
+      <c r="A12" s="16">
         <v>7</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A13" s="14">
@@ -1275,28 +1300,28 @@
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A15" s="30">
+      <c r="A15" s="29">
         <v>10</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A17" s="18">
@@ -1344,49 +1369,49 @@
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A20" s="30">
+      <c r="A20" s="29">
         <v>14</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A21" s="30">
+      <c r="A21" s="29">
         <v>15</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A22" s="30">
+      <c r="A22" s="29">
         <v>16</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A23" s="14">
@@ -1404,19 +1429,19 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A24" s="30">
+      <c r="A24" s="29">
         <v>18</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
       <c r="A25" s="14">
@@ -2104,34 +2129,34 @@
       <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A54" s="30">
+      <c r="A54" s="29">
         <v>26</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A55" s="30">
+      <c r="A55" s="29">
         <v>27</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
     </row>
     <row r="56" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A56" s="18">
@@ -2164,34 +2189,34 @@
       <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A58" s="30">
+      <c r="A58" s="29">
         <v>30</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
     </row>
     <row r="59" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A59" s="30">
+      <c r="A59" s="29">
         <v>31</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C59" s="33" t="s">
+      <c r="C59" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:7" ht="15.6">
       <c r="A60" s="16">
@@ -2211,19 +2236,19 @@
       <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A61" s="30">
+      <c r="A61" s="29">
         <v>33</v>
       </c>
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
     </row>
     <row r="62" spans="1:7" ht="15.6">
       <c r="A62" s="16">
@@ -2331,44 +2356,55 @@
       <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:7" s="13" customFormat="1" ht="15.6">
-      <c r="A69" s="30">
+      <c r="A69" s="29">
         <v>41</v>
       </c>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="30" t="s">
+      <c r="C69" s="29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="B71" s="11" t="s">
+    <row r="70" spans="1:7" ht="15.6">
+      <c r="A70" s="16">
+        <v>42</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" s="36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="B72" s="12" t="s">
+    <row r="78" spans="1:7">
+      <c r="B78" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C78" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="B73" s="7" t="s">
+    <row r="79" spans="1:7">
+      <c r="B79" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C79" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="B74" s="10" t="s">
+    <row r="80" spans="1:7">
+      <c r="B80" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="B75" s="27" t="s">
+    <row r="81" spans="2:2">
+      <c r="B81" s="27" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed 'footer: null' in all editPage. Added AIface template page duplicating from website page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added showing dialogs in AIface config page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
   <si>
     <t>数据总览</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>Binding Management</t>
+  </si>
+  <si>
+    <t>成功, … , message</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2418,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2544,6 +2547,9 @@
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3">

</xml_diff>

<commit_message>
Enabled water AI face page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -808,10 +808,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ81"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1341,20 +1341,20 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A18" s="16">
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A18" s="18">
         <v>12</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" s="9" customFormat="1" ht="15.6">
       <c r="A19" s="18">
@@ -2369,8 +2369,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.6">
-      <c r="A70" s="16">
+    <row r="70" spans="1:7" s="9" customFormat="1" ht="15.6">
+      <c r="A70" s="18">
         <v>42</v>
       </c>
       <c r="B70" s="35" t="s">
@@ -2421,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merged rebate strategy page of Figma and docx. Fixed add dialog in user goup page.
</commit_message>
<xml_diff>
--- a/1.docs/ToDo.xlsx
+++ b/1.docs/ToDo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Ant-Vue\ZCool-live-broadcast-systemdev-\1.docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\ZCool_Ant_FH\ZCool-live-broadcast-systemdev-\1.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="172">
   <si>
     <t>数据总览</t>
   </si>
@@ -543,6 +543,12 @@
   </si>
   <si>
     <t>成功, … , message</t>
+  </si>
+  <si>
+    <t>richedit toolbar wrap</t>
+  </si>
+  <si>
+    <t>activity edit page component</t>
   </si>
 </sst>
 </file>
@@ -805,13 +811,13 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,23 +1097,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AZ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -1122,7 +1128,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -1141,7 +1147,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A4" s="14"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -1154,7 +1160,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A5" s="29"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -1167,7 +1173,7 @@
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A6" s="29"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -1180,7 +1186,7 @@
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A7" s="18">
         <v>3</v>
       </c>
@@ -1195,7 +1201,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A8" s="14">
         <v>4</v>
       </c>
@@ -1210,7 +1216,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A9" s="14">
         <v>5</v>
       </c>
@@ -1229,7 +1235,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A10" s="14"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -1242,7 +1248,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A11" s="14">
         <v>6</v>
       </c>
@@ -1257,22 +1263,22 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" s="11" customFormat="1" ht="15.6">
-      <c r="A12" s="16">
+    <row r="12" spans="1:7" s="27" customFormat="1" ht="15.75">
+      <c r="A12" s="28">
         <v>7</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="15.6">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A13" s="14">
         <v>8</v>
       </c>
@@ -1287,7 +1293,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" ht="15.6">
+    <row r="14" spans="1:7" s="8" customFormat="1" ht="15.75">
       <c r="A14" s="17">
         <v>9</v>
       </c>
@@ -1302,7 +1308,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A15" s="29">
         <v>10</v>
       </c>
@@ -1317,7 +1323,7 @@
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A16" s="29"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -1326,7 +1332,7 @@
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="17" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A17" s="18">
         <v>11</v>
       </c>
@@ -1341,7 +1347,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A18" s="18">
         <v>12</v>
       </c>
@@ -1356,7 +1362,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="19" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A19" s="18">
         <v>13</v>
       </c>
@@ -1371,7 +1377,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A20" s="29">
         <v>14</v>
       </c>
@@ -1386,7 +1392,7 @@
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A21" s="29">
         <v>15</v>
       </c>
@@ -1401,7 +1407,7 @@
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A22" s="29">
         <v>16</v>
       </c>
@@ -1416,7 +1422,7 @@
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -1431,7 +1437,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="24" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A24" s="29">
         <v>18</v>
       </c>
@@ -1446,7 +1452,7 @@
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -1465,7 +1471,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1478,7 +1484,7 @@
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1491,7 +1497,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1504,7 +1510,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1517,7 +1523,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1530,7 +1536,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="31" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -1543,7 +1549,7 @@
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" ht="15.6">
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="15.75">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1556,7 +1562,7 @@
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="33" spans="1:52" s="7" customFormat="1" ht="15.75">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1569,7 +1575,7 @@
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="34" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1627,7 +1633,7 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="7"/>
     </row>
-    <row r="35" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="35" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1685,7 +1691,7 @@
       <c r="AY35" s="7"/>
       <c r="AZ35" s="7"/>
     </row>
-    <row r="36" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="36" spans="1:52" s="7" customFormat="1" ht="15.75">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1698,7 +1704,7 @@
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="37" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1756,7 +1762,7 @@
       <c r="AY37" s="7"/>
       <c r="AZ37" s="7"/>
     </row>
-    <row r="38" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="38" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -1814,7 +1820,7 @@
       <c r="AY38" s="7"/>
       <c r="AZ38" s="7"/>
     </row>
-    <row r="39" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="39" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1872,7 +1878,7 @@
       <c r="AY39" s="7"/>
       <c r="AZ39" s="7"/>
     </row>
-    <row r="40" spans="1:52" s="11" customFormat="1" ht="15.6">
+    <row r="40" spans="1:52" s="11" customFormat="1" ht="15.75">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -1930,7 +1936,7 @@
       <c r="AY40" s="7"/>
       <c r="AZ40" s="7"/>
     </row>
-    <row r="41" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="41" spans="1:52" s="7" customFormat="1" ht="15.75">
       <c r="A41" s="14">
         <v>20</v>
       </c>
@@ -1949,7 +1955,7 @@
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="42" spans="1:52" s="7" customFormat="1" ht="15.75">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -1962,7 +1968,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:52" s="7" customFormat="1" ht="15.6">
+    <row r="43" spans="1:52" s="7" customFormat="1" ht="15.75">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -1975,7 +1981,7 @@
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="1:52" s="12" customFormat="1" ht="15.6">
+    <row r="44" spans="1:52" s="12" customFormat="1" ht="15.75">
       <c r="A44" s="19">
         <v>21</v>
       </c>
@@ -1994,7 +2000,7 @@
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
     </row>
-    <row r="45" spans="1:52" s="9" customFormat="1" ht="15.6">
+    <row r="45" spans="1:52" s="9" customFormat="1" ht="15.75">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
@@ -2007,7 +2013,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
     </row>
-    <row r="46" spans="1:52" s="12" customFormat="1" ht="15.6">
+    <row r="46" spans="1:52" s="12" customFormat="1" ht="15.75">
       <c r="A46" s="19">
         <v>22</v>
       </c>
@@ -2026,7 +2032,7 @@
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
     </row>
-    <row r="47" spans="1:52" s="12" customFormat="1" ht="15.6">
+    <row r="47" spans="1:52" s="12" customFormat="1" ht="15.75">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
@@ -2039,7 +2045,7 @@
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
     </row>
-    <row r="48" spans="1:52" s="12" customFormat="1" ht="15.6">
+    <row r="48" spans="1:52" s="12" customFormat="1" ht="15.75">
       <c r="A48" s="19">
         <v>23</v>
       </c>
@@ -2058,7 +2064,7 @@
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
     </row>
-    <row r="49" spans="1:7" s="12" customFormat="1" ht="15.6">
+    <row r="49" spans="1:7" s="12" customFormat="1" ht="15.75">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
@@ -2071,7 +2077,7 @@
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
     </row>
-    <row r="50" spans="1:7" s="12" customFormat="1" ht="15.6">
+    <row r="50" spans="1:7" s="12" customFormat="1" ht="15.75">
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
@@ -2084,7 +2090,7 @@
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
     </row>
-    <row r="51" spans="1:7" s="12" customFormat="1" ht="15.6">
+    <row r="51" spans="1:7" s="12" customFormat="1" ht="15.75">
       <c r="A51" s="19">
         <v>24</v>
       </c>
@@ -2103,7 +2109,7 @@
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="1:7" s="12" customFormat="1" ht="15.6">
+    <row r="52" spans="1:7" s="12" customFormat="1" ht="15.75">
       <c r="A52" s="19"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
@@ -2116,7 +2122,7 @@
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
     </row>
-    <row r="53" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A53" s="18">
         <v>25</v>
       </c>
@@ -2131,7 +2137,7 @@
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="54" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A54" s="29">
         <v>26</v>
       </c>
@@ -2146,7 +2152,7 @@
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
     </row>
-    <row r="55" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="55" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A55" s="29">
         <v>27</v>
       </c>
@@ -2161,7 +2167,7 @@
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
     </row>
-    <row r="56" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="56" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A56" s="18">
         <v>28</v>
       </c>
@@ -2176,7 +2182,7 @@
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="57" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A57" s="18">
         <v>29</v>
       </c>
@@ -2191,7 +2197,7 @@
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="58" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A58" s="29">
         <v>30</v>
       </c>
@@ -2206,7 +2212,7 @@
       <c r="F58" s="29"/>
       <c r="G58" s="29"/>
     </row>
-    <row r="59" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="59" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A59" s="29">
         <v>31</v>
       </c>
@@ -2221,7 +2227,7 @@
       <c r="F59" s="29"/>
       <c r="G59" s="29"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6">
+    <row r="60" spans="1:7" ht="15.75">
       <c r="A60" s="16">
         <v>32</v>
       </c>
@@ -2238,7 +2244,7 @@
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
     </row>
-    <row r="61" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="61" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A61" s="29">
         <v>33</v>
       </c>
@@ -2253,7 +2259,7 @@
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6">
+    <row r="62" spans="1:7" ht="15.75">
       <c r="A62" s="16">
         <v>34</v>
       </c>
@@ -2268,7 +2274,7 @@
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6">
+    <row r="63" spans="1:7" ht="15.75">
       <c r="A63" s="16">
         <v>35</v>
       </c>
@@ -2283,7 +2289,7 @@
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
     </row>
-    <row r="64" spans="1:7" s="27" customFormat="1" ht="15.6">
+    <row r="64" spans="1:7" s="27" customFormat="1" ht="15.75">
       <c r="A64" s="28">
         <v>36</v>
       </c>
@@ -2298,7 +2304,7 @@
       <c r="F64" s="28"/>
       <c r="G64" s="28"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6">
+    <row r="65" spans="1:7" ht="15.75">
       <c r="A65" s="16">
         <v>37</v>
       </c>
@@ -2313,7 +2319,7 @@
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6">
+    <row r="66" spans="1:7" ht="15.75">
       <c r="A66" s="16">
         <v>38</v>
       </c>
@@ -2328,7 +2334,7 @@
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6">
+    <row r="67" spans="1:7" ht="15.75">
       <c r="A67" s="16">
         <v>39</v>
       </c>
@@ -2343,7 +2349,7 @@
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6">
+    <row r="68" spans="1:7" ht="15.75">
       <c r="A68" s="16">
         <v>40</v>
       </c>
@@ -2358,7 +2364,7 @@
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
     </row>
-    <row r="69" spans="1:7" s="13" customFormat="1" ht="15.6">
+    <row r="69" spans="1:7" s="13" customFormat="1" ht="15.75">
       <c r="A69" s="29">
         <v>41</v>
       </c>
@@ -2369,14 +2375,14 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="70" spans="1:7" s="9" customFormat="1" ht="15.75">
       <c r="A70" s="18">
         <v>42</v>
       </c>
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="C70" s="36" t="s">
+      <c r="C70" s="35" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2421,16 +2427,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="61.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2553,7 +2559,15 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25" s="5"/>

</xml_diff>